<commit_message>
Removed Ufacts and Firefox search
</commit_message>
<xml_diff>
--- a/SeleniumProject/DataSources/TestData.xlsx
+++ b/SeleniumProject/DataSources/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WAPFML\WAPFML_Selenium\SeleniumProject\DataSources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SelWA\SelWA\SeleniumProject\DataSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="7500" windowHeight="1703"/>
+    <workbookView xWindow="0" yWindow="50" windowWidth="7500" windowHeight="1700"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseData" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
     <t>SearchText</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>GoogleNews</t>
   </si>
 </sst>
 </file>
@@ -444,49 +444,49 @@
   <dimension ref="A1:AI21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.53125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="28.796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.796875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="37.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="34.796875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="35.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.53125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="34.796875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="38.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="28.81640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.81640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="37.36328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="34.81640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="35.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="34.81640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="38.08984375" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="28" style="2" customWidth="1"/>
     <col min="14" max="14" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.796875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.53125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="30.796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="35.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27.53125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.81640625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="22.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="35.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="26" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.36328125" style="2" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.19921875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="19.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.1796875" style="2" customWidth="1"/>
     <col min="30" max="30" width="19" style="2" customWidth="1"/>
-    <col min="31" max="31" width="24.53125" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="26.796875" style="2" customWidth="1"/>
+    <col min="31" max="31" width="24.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.81640625" style="2" customWidth="1"/>
     <col min="33" max="33" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="39" max="16384" width="9.1328125" style="2"/>
+    <col min="34" max="35" width="17.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="22.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="22.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="16384" width="9.08984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="7"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -523,7 +523,7 @@
       <c r="AH1" s="3"/>
       <c r="AI1" s="3"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -560,7 +560,7 @@
       <c r="AH2" s="3"/>
       <c r="AI2" s="3"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,7 +582,7 @@
       <c r="X3"/>
       <c r="Y3"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -601,7 +601,7 @@
       <c r="X4"/>
       <c r="Y4"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="G5" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +618,7 @@
       <c r="AH5" s="3"/>
       <c r="AI5" s="3"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -659,7 +659,7 @@
       <c r="AH6" s="3"/>
       <c r="AI6" s="3"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
@@ -676,7 +676,7 @@
       <c r="AH7" s="3"/>
       <c r="AI7" s="3"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
@@ -693,7 +693,7 @@
       <c r="AH8" s="3"/>
       <c r="AI8" s="3"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
       <c r="X9"/>
       <c r="Y9"/>
       <c r="Z9" s="4"/>
@@ -707,7 +707,7 @@
       <c r="AH9" s="3"/>
       <c r="AI9" s="3"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
       <c r="X10" s="4"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="4"/>
@@ -721,7 +721,7 @@
       <c r="AH10" s="3"/>
       <c r="AI10" s="3"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="X11" s="4"/>
       <c r="Z11" s="4"/>
       <c r="AA11" s="3"/>
@@ -734,7 +734,7 @@
       <c r="AH11" s="3"/>
       <c r="AI11" s="3"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
@@ -748,7 +748,7 @@
       <c r="AH12" s="3"/>
       <c r="AI12" s="3"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
@@ -762,7 +762,7 @@
       <c r="AH13" s="3"/>
       <c r="AI13" s="3"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
@@ -776,7 +776,7 @@
       <c r="AH14" s="3"/>
       <c r="AI14" s="3"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
@@ -790,7 +790,7 @@
       <c r="AH15" s="3"/>
       <c r="AI15" s="3"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -827,7 +827,7 @@
       <c r="AH16" s="3"/>
       <c r="AI16" s="3"/>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -864,7 +864,7 @@
       <c r="AH17" s="3"/>
       <c r="AI17" s="3"/>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -901,7 +901,7 @@
       <c r="AH18" s="3"/>
       <c r="AI18" s="3"/>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -938,7 +938,7 @@
       <c r="AH19" s="3"/>
       <c r="AI19" s="3"/>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -975,7 +975,7 @@
       <c r="AH20" s="3"/>
       <c r="AI20" s="3"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>

</xml_diff>